<commit_message>
Implemetação da estrutura das páginas
</commit_message>
<xml_diff>
--- a/esquemas/SPRINT ZERO.xlsx
+++ b/esquemas/SPRINT ZERO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="31995" windowHeight="16485" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="31995" windowHeight="16485" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Histórias" sheetId="5" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="84">
   <si>
     <t>Nome da Tarefa</t>
   </si>
@@ -671,11 +671,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="195144936"/>
-        <c:axId val="195149416"/>
+        <c:axId val="192964896"/>
+        <c:axId val="192965280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="195144936"/>
+        <c:axId val="192964896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -685,7 +685,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195149416"/>
+        <c:crossAx val="192965280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -693,7 +693,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="195149416"/>
+        <c:axId val="192965280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -706,7 +706,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195144936"/>
+        <c:crossAx val="192964896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1053,7 +1053,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,8 +1319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,12 +1439,14 @@
         <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F6" s="3">
         <v>3</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="L6">
         <v>3</v>
       </c>
@@ -1471,6 +1473,9 @@
       <c r="E7" t="s">
         <v>37</v>
       </c>
+      <c r="G7" t="s">
+        <v>56</v>
+      </c>
       <c r="L7">
         <v>4</v>
       </c>
@@ -1521,12 +1526,14 @@
         <v>7</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F9" s="3">
         <v>8</v>
       </c>
-      <c r="G9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="L9">
         <v>6</v>
       </c>
@@ -1544,6 +1551,9 @@
       <c r="E10" t="s">
         <v>37</v>
       </c>
+      <c r="G10" t="s">
+        <v>56</v>
+      </c>
       <c r="L10">
         <v>7</v>
       </c>
@@ -1588,12 +1598,14 @@
         <v>7</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F12" s="3">
         <v>3</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1608,6 +1620,9 @@
       <c r="E13" t="s">
         <v>37</v>
       </c>
+      <c r="G13" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="14" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1646,12 +1661,14 @@
         <v>7</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F15" s="3">
         <v>5</v>
       </c>
-      <c r="G15" s="3"/>
+      <c r="G15" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1704,13 +1721,13 @@
         <v>7</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F18" s="3">
         <v>8</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1726,6 +1743,9 @@
       <c r="E19" t="s">
         <v>37</v>
       </c>
+      <c r="G19" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -1792,7 +1812,9 @@
       <c r="F22" s="3">
         <v>8</v>
       </c>
-      <c r="G22" s="3"/>
+      <c r="G22" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -1806,6 +1828,9 @@
       </c>
       <c r="E23" t="s">
         <v>37</v>
+      </c>
+      <c r="G23" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1901,8 +1926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
comentando o codigo das paginas, ainda falta o css
</commit_message>
<xml_diff>
--- a/esquemas/SPRINT ZERO.xlsx
+++ b/esquemas/SPRINT ZERO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="31995" windowHeight="16485" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="31995" windowHeight="16485" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Histórias" sheetId="5" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="85">
   <si>
     <t>Nome da Tarefa</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t>Nº Item</t>
+  </si>
+  <si>
+    <t>Soma</t>
   </si>
 </sst>
 </file>
@@ -332,7 +335,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,6 +370,24 @@
       <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
       </patternFill>
     </fill>
   </fills>
@@ -444,7 +465,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -470,6 +491,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -599,6 +635,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -632,31 +698,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>90</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -740,16 +806,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>7937</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>39290</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>582704</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>36909</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1061,7 +1127,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,18 +1139,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:4" ht="5.0999999999999996" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1327,8 +1393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1342,22 +1408,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
       <c r="L2" t="s">
         <v>40</v>
       </c>
@@ -1412,7 +1478,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="F5" s="2">
         <v>5</v>
@@ -1447,7 +1513,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="F6" s="3">
         <v>3</v>
@@ -1479,7 +1545,10 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
       </c>
       <c r="G7" t="s">
         <v>56</v>
@@ -1534,10 +1603,10 @@
         <v>7</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="F9" s="3">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>58</v>
@@ -1557,7 +1626,10 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
       </c>
       <c r="G10" t="s">
         <v>56</v>
@@ -1606,7 +1678,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="F12" s="3">
         <v>3</v>
@@ -1626,7 +1698,10 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
       </c>
       <c r="G13" t="s">
         <v>56</v>
@@ -1646,7 +1721,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="F14" s="2">
         <v>5</v>
@@ -1669,7 +1744,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="F15" s="3">
         <v>5</v>
@@ -1689,7 +1764,10 @@
         <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
       </c>
       <c r="G16" t="s">
         <v>56</v>
@@ -1709,7 +1787,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" s="2">
         <v>5</v>
@@ -1732,10 +1810,10 @@
         <v>7</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="F18" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>58</v>
@@ -1752,7 +1830,10 @@
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>39</v>
+        <v>8</v>
+      </c>
+      <c r="F19">
+        <v>5</v>
       </c>
       <c r="G19" t="s">
         <v>56</v>
@@ -1874,7 +1955,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3">
         <f>SUM(F5:F24)</f>
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="G25" s="3"/>
     </row>
@@ -1937,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,21 +2035,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
       <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
     </row>
     <row r="3" spans="1:17" ht="5.0999999999999996" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2022,224 +2103,589 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
+      <c r="A5" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>3</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0</v>
+      </c>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
+    <row r="6" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="3">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0</v>
+      </c>
       <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="A7" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <v>3</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0</v>
+      </c>
       <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
+      <c r="A8" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="3">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>5</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0</v>
+      </c>
       <c r="Q8" s="3"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+    <row r="9" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="2">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>5</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2">
+        <v>0</v>
+      </c>
       <c r="Q9" s="2"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
+      <c r="A10" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="3">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3">
+        <v>4</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0</v>
+      </c>
+      <c r="O10" s="3">
+        <v>0</v>
+      </c>
+      <c r="P10" s="3">
+        <v>0</v>
+      </c>
       <c r="Q10" s="3"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
+    <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="2">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>4</v>
+      </c>
+      <c r="I11" s="2">
+        <v>4</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2">
+        <v>0</v>
+      </c>
       <c r="Q11" s="2"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
+      <c r="A12" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="3">
+        <v>3</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="15">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
+      <c r="J12" s="3">
+        <v>3</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0</v>
+      </c>
+      <c r="O12" s="3">
+        <v>0</v>
+      </c>
+      <c r="P12" s="3">
+        <v>0</v>
+      </c>
       <c r="Q12" s="3"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
+      <c r="A13" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="2">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2</v>
+      </c>
+      <c r="G13" s="16">
+        <v>0</v>
+      </c>
+      <c r="H13" s="16">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>3</v>
+      </c>
+      <c r="L13" s="2">
+        <v>2</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0</v>
+      </c>
       <c r="Q13" s="2"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
+      <c r="A14" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="3">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="15">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0</v>
+      </c>
+      <c r="L14" s="3">
+        <v>5</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0</v>
+      </c>
+      <c r="N14" s="3">
+        <v>0</v>
+      </c>
+      <c r="O14" s="3">
+        <v>0</v>
+      </c>
+      <c r="P14" s="3">
+        <v>0</v>
+      </c>
       <c r="Q14" s="3"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
+      <c r="A15" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="2">
+        <v>5</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2">
+        <v>4</v>
+      </c>
+      <c r="G15" s="16">
+        <v>0</v>
+      </c>
+      <c r="H15" s="16">
+        <v>0</v>
+      </c>
+      <c r="I15" s="16">
+        <v>0</v>
+      </c>
+      <c r="J15" s="16">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1</v>
+      </c>
+      <c r="M15" s="2">
+        <v>2</v>
+      </c>
+      <c r="N15" s="2">
+        <v>1</v>
+      </c>
+      <c r="O15" s="2">
+        <v>2</v>
+      </c>
+      <c r="P15" s="2">
+        <v>0</v>
+      </c>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
+    <row r="16" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="3">
+        <v>5</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="3">
+        <v>2</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0</v>
+      </c>
+      <c r="L16" s="3">
+        <v>0</v>
+      </c>
+      <c r="M16" s="3">
+        <v>0</v>
+      </c>
+      <c r="N16" s="3">
+        <v>0</v>
+      </c>
+      <c r="O16" s="3">
+        <v>0</v>
+      </c>
+      <c r="P16" s="3">
+        <v>5</v>
+      </c>
       <c r="Q16" s="3"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="2">
+        <f>SUM(B5:B16)</f>
+        <v>55</v>
+      </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -2315,29 +2761,89 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
+      <c r="G21" s="2">
+        <f t="shared" ref="G21:P21" si="0">SUM(G5:G20)</f>
+        <v>20</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N21" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O21" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P21" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="Q21" s="2"/>
     </row>
     <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
+      <c r="G22">
+        <f>SUM(E23,-G21)</f>
+        <v>35</v>
+      </c>
+      <c r="H22">
+        <f>SUM(G22,-H21)</f>
+        <v>27</v>
+      </c>
+      <c r="I22">
+        <f>SUM(H22,-I21)</f>
+        <v>23</v>
+      </c>
+      <c r="J22">
+        <f t="shared" ref="J22:P22" si="1">SUM(I22,-J21)</f>
+        <v>20</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
       <c r="Q22" s="10"/>
     </row>
     <row r="23" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2347,42 +2853,44 @@
       <c r="D23" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="7">
-        <v>100</v>
+      <c r="E23" s="20">
+        <f>SUM(B5:B16)</f>
+        <v>55</v>
       </c>
       <c r="F23" s="9">
         <v>100</v>
       </c>
-      <c r="G23" s="7">
-        <v>90</v>
-      </c>
-      <c r="H23" s="7">
-        <v>80</v>
-      </c>
-      <c r="I23" s="7">
-        <v>70</v>
-      </c>
-      <c r="J23" s="7">
-        <v>60</v>
-      </c>
-      <c r="K23" s="7">
-        <v>50</v>
-      </c>
-      <c r="L23" s="7">
-        <v>40</v>
-      </c>
-      <c r="M23" s="7">
-        <v>30</v>
-      </c>
-      <c r="N23" s="7">
-        <v>20</v>
-      </c>
-      <c r="O23" s="7">
-        <v>10</v>
-      </c>
-      <c r="P23" s="7">
-        <v>0</v>
-      </c>
+      <c r="G23" s="21">
+        <v>49.5</v>
+      </c>
+      <c r="H23" s="21">
+        <v>44</v>
+      </c>
+      <c r="I23" s="21">
+        <v>38.5</v>
+      </c>
+      <c r="J23" s="21">
+        <v>33</v>
+      </c>
+      <c r="K23" s="21">
+        <v>27.5</v>
+      </c>
+      <c r="L23" s="21">
+        <v>22</v>
+      </c>
+      <c r="M23" s="21">
+        <v>16.5</v>
+      </c>
+      <c r="N23" s="21">
+        <v>11</v>
+      </c>
+      <c r="O23" s="21">
+        <v>5.5</v>
+      </c>
+      <c r="P23" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="20"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C24" s="7" t="s">

</xml_diff>